<commit_message>
ajout en cours d'un projectile façon Cappy
</commit_message>
<xml_diff>
--- a/Super_Retro_World_v3/Planning_2018_v2.xlsx
+++ b/Super_Retro_World_v3/Planning_2018_v2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995"/>
@@ -256,7 +256,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="65">
   <si>
     <t>Débuter au</t>
   </si>
@@ -448,6 +448,9 @@
   </si>
   <si>
     <t>Déplacements</t>
+  </si>
+  <si>
+    <t>Item à récupérer</t>
   </si>
 </sst>
 </file>
@@ -15566,21 +15569,7 @@
     <cellStyle name="差_Suivi postes et candidats " xfId="3121"/>
     <cellStyle name="標準_CAR FLOW 2004 84 for A3 20040907 &amp; BUDGET B2005 " xfId="3122"/>
   </cellStyles>
-  <dxfs count="57">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="56">
     <dxf>
       <font>
         <b/>
@@ -15945,6 +15934,13 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF2C6129"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -19008,7 +19004,7 @@
   <dimension ref="A1:GJ43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19:F19"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" outlineLevelRow="2"/>
@@ -23592,10 +23588,14 @@
         <v>12</v>
       </c>
       <c r="D9" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="24"/>
-      <c r="F9" s="25"/>
+        <v>64</v>
+      </c>
+      <c r="E9" s="24">
+        <v>43235</v>
+      </c>
+      <c r="F9" s="25">
+        <v>43266</v>
+      </c>
       <c r="G9" s="20">
         <f t="shared" ca="1" si="6"/>
         <v>0</v>
@@ -23774,131 +23774,131 @@
       </c>
       <c r="AY9" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ9" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA9" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB9" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC9" s="21">
         <f t="shared" ref="BC9:BR24" ca="1" si="17">IF(AND(BC$4&gt;=$E9,BC$4&lt;=$F9),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR9" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS9" s="21">
         <f t="shared" ref="BS9:CH24" ca="1" si="18">IF(AND(BS$4&gt;=$E9,BS$4&lt;=$F9),1,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD9" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CE9" s="21">
         <f t="shared" ca="1" si="18"/>
@@ -29635,10 +29635,10 @@
         <v>57</v>
       </c>
       <c r="E17" s="24">
+        <v>43221</v>
+      </c>
+      <c r="F17" s="25">
         <v>43252</v>
-      </c>
-      <c r="F17" s="25">
-        <v>43266</v>
       </c>
       <c r="G17" s="20">
         <f t="shared" ca="1" si="6"/>
@@ -29762,127 +29762,127 @@
       </c>
       <c r="AK17" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL17" s="21">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AT17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB17" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP17" s="21">
         <f t="shared" ca="1" si="17"/>
@@ -29890,59 +29890,59 @@
       </c>
       <c r="BQ17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BR17" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BT17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BV17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BX17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BY17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CA17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CC17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CD17" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CE17" s="21">
         <f t="shared" ca="1" si="18"/>
@@ -30386,7 +30386,7 @@
         <v>60</v>
       </c>
       <c r="E18" s="24">
-        <v>43266</v>
+        <v>43235</v>
       </c>
       <c r="F18" s="25">
         <v>43282</v>
@@ -30569,127 +30569,127 @@
       </c>
       <c r="AY18" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AZ18" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA18" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB18" s="21">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BC18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BD18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BE18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BG18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BI18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BJ18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BK18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BQ18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BR18" s="21">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BT18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BV18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BX18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BY18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CA18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CC18" s="21">
         <f t="shared" ca="1" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CD18" s="21">
         <f t="shared" ca="1" si="18"/>
@@ -48612,282 +48612,282 @@
     <mergeCell ref="X2:AN2"/>
   </mergeCells>
   <conditionalFormatting sqref="G5:GG41">
-    <cfRule type="expression" dxfId="56" priority="56">
+    <cfRule type="expression" dxfId="55" priority="56">
       <formula>G$4=EOMONTH(G$4,-1)+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:GG4">
-    <cfRule type="expression" dxfId="55" priority="55">
+    <cfRule type="expression" dxfId="54" priority="55">
       <formula>G$4=EOMONTH(G$4,-1)+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5:B5 D5:CK5 GD5:XFD5">
-    <cfRule type="cellIs" dxfId="54" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="54" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6:B6 A11:B11 A15:B15 D15:CK15 D11:CK11 D6:CK6 GD15:XFD15 GD11:XFD11 GD6:XFD6 GD13:XFD13">
-    <cfRule type="cellIs" dxfId="53" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="53" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:B10 A12:B12 A16:B19 D12:CK12 D7:CK10 GD16:XFD19 GD12:XFD12 GD7:XFD10 GD14:XFD14 D16:CK19">
-    <cfRule type="cellIs" dxfId="1" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="52" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:B20 D20:CK20 GD20:XFD20">
-    <cfRule type="cellIs" dxfId="52" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="51" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:B21 D21:CK21 GD21:XFD21">
-    <cfRule type="cellIs" dxfId="51" priority="50" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="50" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A22:B25 D22:CK25 GD22:XFD25">
-    <cfRule type="cellIs" dxfId="50" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="49" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26 D26:CK26 GD26:XFD26">
-    <cfRule type="cellIs" dxfId="49" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 D27:CK27 GD27:XFD27">
-    <cfRule type="cellIs" dxfId="48" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="46" priority="47" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B31 D28:CK31 GD28:XFD31">
-    <cfRule type="cellIs" dxfId="47" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A32:B32 D32:CK32 GD32:XFD32">
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="45" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33 D33:CK33 GD33:XFD33">
-    <cfRule type="cellIs" dxfId="45" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="44" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A34:B37 D34:CK37 GD34:XFD37">
-    <cfRule type="cellIs" dxfId="44" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:B38 D38:CK38 GD38:XFD38">
-    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A39:B39 D39:CK39 GD39:XFD39">
-    <cfRule type="cellIs" dxfId="42" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="41" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A40:B41 D40:CK41 GD40:XFD41">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="40" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14:B14 D14:CK14">
-    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="38" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A13:B13 D13:CK13">
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="39" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL14:GC14">
-    <cfRule type="cellIs" dxfId="38" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL5:GC5">
-    <cfRule type="cellIs" dxfId="37" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL15:GC15 CL11:GC11 CL6:GC6">
-    <cfRule type="cellIs" dxfId="36" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="36" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL16:GC19 CL12:GC12 CL7:GC10">
-    <cfRule type="cellIs" dxfId="35" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="35" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL20:GC20">
-    <cfRule type="cellIs" dxfId="34" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL21:GC21">
-    <cfRule type="cellIs" dxfId="33" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="33" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL22:GC25">
-    <cfRule type="cellIs" dxfId="32" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="32" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL26:GC26">
-    <cfRule type="cellIs" dxfId="31" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL27:GC27">
-    <cfRule type="cellIs" dxfId="30" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="30" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL28:GC31">
-    <cfRule type="cellIs" dxfId="29" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="29" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL32:GC32">
-    <cfRule type="cellIs" dxfId="28" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL33:GC33">
-    <cfRule type="cellIs" dxfId="27" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="27" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL34:GC37">
-    <cfRule type="cellIs" dxfId="26" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="26" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL38:GC38">
-    <cfRule type="cellIs" dxfId="25" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL39:GC39">
-    <cfRule type="cellIs" dxfId="24" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="24" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL40:GC41">
-    <cfRule type="cellIs" dxfId="23" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="23" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CL13:GC13">
-    <cfRule type="cellIs" dxfId="22" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="22" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="20" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C15 C11 C6">
-    <cfRule type="cellIs" dxfId="20" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16:C19 C12 C7:C10">
-    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="18" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="cellIs" dxfId="18" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="17" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21">
-    <cfRule type="cellIs" dxfId="17" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C22:C25">
-    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="15" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="cellIs" dxfId="15" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C31">
-    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C32">
-    <cfRule type="cellIs" dxfId="12" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C34:C37">
-    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C38">
-    <cfRule type="cellIs" dxfId="9" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C39">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C40:C41">
-    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C14">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:GG41">
-    <cfRule type="expression" dxfId="4" priority="3">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>G$4=TODAY()</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3:GG3">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>G$4=EOMONTH(G$4,-1)+1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5:D41">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND($E5&lt;=TODAY(),$F5&gt;=TODAY())</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>